<commit_message>
changed to 1.5mm RGBLEDs because cheaper
</commit_message>
<xml_diff>
--- a/pcb/BOM.xlsx
+++ b/pcb/BOM.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="142">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -160,10 +160,10 @@
     <t xml:space="preserve">D210,D211,D232,D258,D250,D249,D261,D252,D227,D200,D221,D231,D206,D201,D233,D253,D208,D255,D254,D251,D228,D212,D244,D263,D204,D219,D218,D225,D238,D241,D246,D224,D262,D240,D229,D245,D215,D226,D213,D239,D202,D248,D257,D230,D220,D222,D243,D205,D207,D223,D235,D260,D209,D256,D247,D236,D242,D237,D216,D214,D203,D259,D234,D217</t>
   </si>
   <si>
-    <t xml:space="preserve">SMD-LX0707RGB-TR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.co.uk/en/products/detail/lumex-opto-components-inc/SMD-LX0707RGB-TR/9858268</t>
+    <t xml:space="preserve">IN-PI15TAT5R5G5B </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.co.uk/en/products/detail/inolux/IN-PI15TAT5R5G5B/14555725</t>
   </si>
   <si>
     <t xml:space="preserve">IC1</t>
@@ -283,7 +283,7 @@
     <t xml:space="preserve">5.1k</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERA-2AEB512X/1706022</t>
+    <t xml:space="preserve">https://www.digikey.co.uk/en/products/detail/yageo/RC0402FR-075K1L/726624</t>
   </si>
   <si>
     <t xml:space="preserve">R203</t>
@@ -292,7 +292,7 @@
     <t xml:space="preserve">2.5k</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERA-2AEB2491X/2026087</t>
+    <t xml:space="preserve">https://www.digikey.co.uk/en/products/detail/yageo/RC0402FR-072K49L/2827582</t>
   </si>
   <si>
     <t xml:space="preserve">R204,R105</t>
@@ -455,7 +455,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -475,6 +475,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -519,13 +525,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -544,6 +562,8 @@
   <dxfs count="2">
     <dxf>
       <font>
+        <name val="Arial"/>
+        <family val="2"/>
         <b val="0"/>
         <i val="0"/>
         <color rgb="FF006600"/>
@@ -557,6 +577,8 @@
     </dxf>
     <dxf>
       <font>
+        <name val="Arial"/>
+        <family val="2"/>
         <b val="0"/>
         <i val="0"/>
         <color rgb="FFCC0000"/>
@@ -640,12 +662,12 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
+      <selection pane="topLeft" activeCell="I52" activeCellId="0" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.38"/>
@@ -842,6 +864,9 @@
       <c r="H9" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="I9" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -981,7 +1006,7 @@
       <c r="B17" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D17" s="0" t="s">
@@ -990,14 +1015,17 @@
       <c r="E17" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="3" t="s">
         <v>46</v>
       </c>
       <c r="G17" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="H17" s="4" t="s">
         <v>47</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,6 +1172,9 @@
       <c r="H25" s="0" t="s">
         <v>71</v>
       </c>
+      <c r="I25" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -1187,6 +1218,9 @@
       <c r="H27" s="0" t="s">
         <v>77</v>
       </c>
+      <c r="I27" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -1213,6 +1247,9 @@
       <c r="H28" s="0" t="s">
         <v>79</v>
       </c>
+      <c r="I28" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -1239,8 +1276,11 @@
       <c r="H29" s="0" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I29" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>27</v>
       </c>
@@ -1305,6 +1345,9 @@
       <c r="H32" s="0" t="s">
         <v>87</v>
       </c>
+      <c r="I32" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -1331,8 +1374,11 @@
       <c r="H33" s="0" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I33" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>24</v>
       </c>
@@ -1448,6 +1494,9 @@
       <c r="H39" s="0" t="s">
         <v>102</v>
       </c>
+      <c r="I39" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -1473,6 +1522,9 @@
       </c>
       <c r="H40" s="0" t="s">
         <v>106</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,6 +1552,9 @@
       <c r="H41" s="0" t="s">
         <v>110</v>
       </c>
+      <c r="I41" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -1539,10 +1594,10 @@
       <c r="A44" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="5" t="s">
         <v>116</v>
       </c>
       <c r="D44" s="0" t="s">
@@ -1559,6 +1614,9 @@
       </c>
       <c r="H44" s="0" t="s">
         <v>118</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1578,7 +1636,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>15</v>
       </c>
@@ -1626,6 +1684,9 @@
       <c r="H47" s="0" t="s">
         <v>127</v>
       </c>
+      <c r="I47" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -1652,6 +1713,9 @@
       <c r="H48" s="0" t="s">
         <v>131</v>
       </c>
+      <c r="I48" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -1678,6 +1742,9 @@
       <c r="H49" s="0" t="s">
         <v>135</v>
       </c>
+      <c r="I49" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -1714,7 +1781,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D1:D1048576 I2:J51">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="x" dxfId="0">
       <formula>NOT(ISERROR(SEARCH("x",D1)))</formula>
     </cfRule>
@@ -1722,6 +1789,9 @@
       <formula>ISERROR(SEARCH("x",D1))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="H17" r:id="rId1" display="https://www.digikey.co.uk/en/products/detail/inolux/IN-PI15TAT5R5G5B/14555725"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>